<commit_message>
backin up beep beep beep
</commit_message>
<xml_diff>
--- a/Literature mapping/evaluation cards.xlsx
+++ b/Literature mapping/evaluation cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Thesis2021\Literature mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D83D48-ECBD-4CF7-BED6-7D8134D7A79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC94E3-AD1E-48F2-807F-49BD21B094AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30555" yWindow="-16965" windowWidth="14400" windowHeight="7365" xr2:uid="{0571A6F9-7A2C-49A8-A015-CDF9129AD4D1}"/>
+    <workbookView xWindow="-21195" yWindow="-21555" windowWidth="15510" windowHeight="20580" xr2:uid="{0571A6F9-7A2C-49A8-A015-CDF9129AD4D1}"/>
   </bookViews>
   <sheets>
     <sheet name="3" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'1'!$B$1:$C$111</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2'!$B$1:$C$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3'!$B$1:$C$210</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3'!$B$1:$C$295</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="175">
   <si>
     <t>Study ID            </t>
   </si>
@@ -631,6 +631,12 @@
   </si>
   <si>
     <t>MPS, MetaEdit+, WebGME, GEMS, sirius,Xtext, MS DSL ToolsMelange, GME*</t>
+  </si>
+  <si>
+    <t>Javardise (Research Project)</t>
+  </si>
+  <si>
+    <t>ALF (Xtext) + Valkyrie (GMF)</t>
   </si>
 </sst>
 </file>
@@ -1119,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293AA2FC-3EF2-4F89-B916-7D2D989016C7}">
   <dimension ref="B1:S295"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F207" sqref="F207"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F258" sqref="F258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2289,7 +2295,9 @@
       <c r="B149" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C149" s="7"/>
+      <c r="C149" s="7" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="150" spans="2:15" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B150" s="8" t="s">
@@ -2363,7 +2371,9 @@
       <c r="B159" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C159" s="7"/>
+      <c r="C159" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="160" spans="2:15" ht="21.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B160" s="8" t="s">
@@ -3511,6 +3521,7 @@
       <c r="E295" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:C295" xr:uid="{293AA2FC-3EF2-4F89-B916-7D2D989016C7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
@@ -3764,7 +3775,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
@@ -4206,7 +4217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B53" s="6" t="s">
         <v>1</v>
       </c>
@@ -4377,7 +4388,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B66" s="6" t="s">
         <v>4</v>
       </c>
@@ -4589,7 +4600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B83" s="6" t="s">
         <v>1</v>
       </c>
@@ -5270,7 +5281,7 @@
       <c r="M132" s="2"/>
       <c r="O132" s="5"/>
     </row>
-    <row r="133" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B133" s="6" t="s">
         <v>1</v>
       </c>
@@ -5466,7 +5477,7 @@
       </c>
       <c r="E148" s="5"/>
     </row>
-    <row r="149" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B149" s="6" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
push just in case
</commit_message>
<xml_diff>
--- a/Literature mapping/evaluation cards.xlsx
+++ b/Literature mapping/evaluation cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Thesis2021\Literature mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC94E3-AD1E-48F2-807F-49BD21B094AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05618D82-0B9D-44DA-8138-F4F21909BAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21195" yWindow="-21555" windowWidth="15510" windowHeight="20580" xr2:uid="{0571A6F9-7A2C-49A8-A015-CDF9129AD4D1}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="13400" windowHeight="10800" xr2:uid="{0571A6F9-7A2C-49A8-A015-CDF9129AD4D1}"/>
   </bookViews>
   <sheets>
     <sheet name="3" sheetId="3" r:id="rId1"/>
@@ -1123,10 +1123,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293AA2FC-3EF2-4F89-B916-7D2D989016C7}">
-  <dimension ref="B1:S295"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B2:S295"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A244" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F258" sqref="F258"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1152,8 +1153,7 @@
     <col min="20" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1225,11 +1225,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>2</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>7</v>
       </c>
@@ -1301,11 +1301,11 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1325,7 @@
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>3</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>4</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>5</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
         <v>6</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
         <v>7</v>
       </c>
@@ -1395,10 +1395,10 @@
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
         <v>1</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
         <v>2</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6" t="s">
         <v>4</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" s="6" t="s">
         <v>7</v>
       </c>
@@ -1470,8 +1470,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" s="3" t="s">
         <v>0</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
         <v>2</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
         <v>3</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>4</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" s="6" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" s="6" t="s">
         <v>7</v>
       </c>
@@ -1543,11 +1543,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" s="12"/>
       <c r="C51" s="13"/>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" s="6" t="s">
         <v>1</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" s="6" t="s">
         <v>2</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" s="6" t="s">
         <v>3</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" s="6" t="s">
         <v>4</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B57" s="6" t="s">
         <v>5</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B58" s="6" t="s">
         <v>6</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B59" s="6" t="s">
         <v>7</v>
       </c>
@@ -1619,11 +1619,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="E61" s="12"/>
       <c r="F61" s="13"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>0</v>
       </c>
@@ -1633,7 +1633,7 @@
       <c r="E62" s="12"/>
       <c r="F62" s="13"/>
     </row>
-    <row r="63" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B63" s="6" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="E63" s="12"/>
       <c r="F63" s="13"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="B64" s="6" t="s">
         <v>2</v>
       </c>
@@ -1653,7 +1653,7 @@
       <c r="E64" s="12"/>
       <c r="F64" s="13"/>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B65" s="6" t="s">
         <v>3</v>
       </c>
@@ -1663,7 +1663,7 @@
       <c r="E65" s="12"/>
       <c r="F65" s="13"/>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B66" s="6" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1675,7 @@
       <c r="M66" s="2"/>
       <c r="O66" s="5"/>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" s="6" t="s">
         <v>5</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="E67" s="12"/>
       <c r="F67" s="13"/>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B68" s="6" t="s">
         <v>6</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="E68" s="12"/>
       <c r="F68" s="13"/>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" s="6" t="s">
         <v>7</v>
       </c>
@@ -1715,8 +1715,8 @@
       <c r="E70" s="12"/>
       <c r="F70" s="13"/>
     </row>
-    <row r="71" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:15" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72" s="3" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" s="6" t="s">
         <v>1</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74" s="6" t="s">
         <v>2</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" s="6" t="s">
         <v>3</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" s="6" t="s">
         <v>4</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B77" s="6" t="s">
         <v>5</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78" s="6" t="s">
         <v>6</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79" s="6" t="s">
         <v>7</v>
       </c>
@@ -1788,8 +1788,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:15" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="82" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>0</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B83" s="6" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84" s="6" t="s">
         <v>2</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85" s="6" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" s="6" t="s">
         <v>4</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="M86" s="2"/>
       <c r="O86" s="5"/>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87" s="6" t="s">
         <v>5</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" s="6" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" s="6" t="s">
         <v>7</v>
       </c>
@@ -1863,8 +1863,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="2:15" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:15" ht="10.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" s="3" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" s="6" t="s">
         <v>1</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" s="6" t="s">
         <v>2</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" s="6" t="s">
         <v>3</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" s="6" t="s">
         <v>4</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" s="6" t="s">
         <v>5</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B98" s="6" t="s">
         <v>6</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99" s="6" t="s">
         <v>7</v>
       </c>
@@ -1936,8 +1936,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="101" spans="2:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:15" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="102" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B102" s="3" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B103" s="6" t="s">
         <v>1</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B104" s="6" t="s">
         <v>2</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B105" s="6" t="s">
         <v>3</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B106" s="6" t="s">
         <v>4</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="M106" s="2"/>
       <c r="O106" s="5"/>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B107" s="6" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="108" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B108" s="6" t="s">
         <v>6</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B109" s="6" t="s">
         <v>7</v>
       </c>
@@ -2011,8 +2011,8 @@
         <v>142</v>
       </c>
     </row>
-    <row r="111" spans="2:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:15" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="112" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B112" s="3" t="s">
         <v>0</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B113" s="6" t="s">
         <v>1</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B114" s="6" t="s">
         <v>2</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B115" s="6" t="s">
         <v>3</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B116" s="6" t="s">
         <v>4</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B117" s="6" t="s">
         <v>5</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B118" s="6" t="s">
         <v>6</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="119" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B119" s="6" t="s">
         <v>7</v>
       </c>
@@ -2084,8 +2084,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="121" spans="2:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="122" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:15" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="122" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B122" s="3" t="s">
         <v>0</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B123" s="6" t="s">
         <v>1</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B124" s="6" t="s">
         <v>2</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="125" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B125" s="6" t="s">
         <v>3</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="126" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B126" s="6" t="s">
         <v>4</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="M126" s="2"/>
       <c r="O126" s="5"/>
     </row>
-    <row r="127" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B127" s="6" t="s">
         <v>5</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="128" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B128" s="6" t="s">
         <v>6</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B129" s="6" t="s">
         <v>7</v>
       </c>
@@ -2159,8 +2159,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:3" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="132" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B132" s="3" t="s">
         <v>0</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B133" s="6" t="s">
         <v>1</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B134" s="6" t="s">
         <v>2</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B135" s="6" t="s">
         <v>3</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B136" s="6" t="s">
         <v>4</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B137" s="6" t="s">
         <v>5</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B138" s="6" t="s">
         <v>6</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B139" s="6" t="s">
         <v>7</v>
       </c>
@@ -2232,8 +2232,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="141" spans="2:3" ht="26.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:3" ht="26.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B142" s="3" t="s">
         <v>0</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="143" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:3" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B143" s="6" t="s">
         <v>1</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B144" s="6" t="s">
         <v>2</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="145" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B145" s="6" t="s">
         <v>3</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B146" s="6" t="s">
         <v>4</v>
       </c>
@@ -2275,7 +2275,7 @@
       <c r="M146" s="2"/>
       <c r="O146" s="5"/>
     </row>
-    <row r="147" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B147" s="6" t="s">
         <v>5</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="148" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B148" s="6" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="149" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B149" s="6" t="s">
         <v>7</v>
       </c>
@@ -2307,11 +2307,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B151" s="12"/>
       <c r="C151" s="13"/>
     </row>
-    <row r="152" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B152" s="3" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B153" s="6" t="s">
         <v>1</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="154" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B154" s="6" t="s">
         <v>2</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="155" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B155" s="6" t="s">
         <v>3</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="156" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B156" s="6" t="s">
         <v>4</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="157" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B157" s="6" t="s">
         <v>5</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="158" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B158" s="6" t="s">
         <v>6</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="159" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B159" s="6" t="s">
         <v>7</v>
       </c>
@@ -2383,11 +2383,11 @@
         <v>147</v>
       </c>
     </row>
-    <row r="161" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="E161" s="12"/>
       <c r="F161" s="13"/>
     </row>
-    <row r="162" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B162" s="3" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="E162" s="12"/>
       <c r="F162" s="13"/>
     </row>
-    <row r="163" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B163" s="6" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2407,7 @@
       <c r="E163" s="12"/>
       <c r="F163" s="13"/>
     </row>
-    <row r="164" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B164" s="6" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2417,7 @@
       <c r="E164" s="12"/>
       <c r="F164" s="13"/>
     </row>
-    <row r="165" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B165" s="6" t="s">
         <v>3</v>
       </c>
@@ -2429,7 +2429,7 @@
       <c r="M165" s="2"/>
       <c r="O165" s="5"/>
     </row>
-    <row r="166" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B166" s="6" t="s">
         <v>4</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="E166" s="12"/>
       <c r="F166" s="13"/>
     </row>
-    <row r="167" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B167" s="6" t="s">
         <v>5</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="13"/>
     </row>
-    <row r="168" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B168" s="6" t="s">
         <v>6</v>
       </c>
@@ -2459,7 +2459,7 @@
       <c r="E168" s="12"/>
       <c r="F168" s="13"/>
     </row>
-    <row r="169" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B169" s="6" t="s">
         <v>7</v>
       </c>
@@ -2479,11 +2479,11 @@
       <c r="E170" s="12"/>
       <c r="F170" s="13"/>
     </row>
-    <row r="171" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B171" s="12"/>
       <c r="C171" s="13"/>
     </row>
-    <row r="172" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B172" s="3" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B173" s="6" t="s">
         <v>1</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="174" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B174" s="6" t="s">
         <v>2</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="175" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B175" s="6" t="s">
         <v>3</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="176" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B176" s="6" t="s">
         <v>4</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="177" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B177" s="6" t="s">
         <v>5</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="178" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B178" s="6" t="s">
         <v>6</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="179" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B179" s="6" t="s">
         <v>7</v>
       </c>
@@ -2555,11 +2555,11 @@
         <v>149</v>
       </c>
     </row>
-    <row r="181" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B181" s="12"/>
       <c r="C181" s="13"/>
     </row>
-    <row r="182" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B182" s="3" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="E182" s="12"/>
       <c r="F182" s="13"/>
     </row>
-    <row r="183" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B183" s="6" t="s">
         <v>1</v>
       </c>
@@ -2579,7 +2579,7 @@
       <c r="E183" s="12"/>
       <c r="F183" s="13"/>
     </row>
-    <row r="184" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B184" s="6" t="s">
         <v>2</v>
       </c>
@@ -2589,7 +2589,7 @@
       <c r="E184" s="12"/>
       <c r="F184" s="13"/>
     </row>
-    <row r="185" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B185" s="6" t="s">
         <v>3</v>
       </c>
@@ -2601,7 +2601,7 @@
       <c r="M185" s="2"/>
       <c r="O185" s="5"/>
     </row>
-    <row r="186" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B186" s="6" t="s">
         <v>4</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="E186" s="12"/>
       <c r="F186" s="13"/>
     </row>
-    <row r="187" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="187" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B187" s="6" t="s">
         <v>5</v>
       </c>
@@ -2621,7 +2621,7 @@
       <c r="E187" s="12"/>
       <c r="F187" s="13"/>
     </row>
-    <row r="188" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B188" s="6" t="s">
         <v>6</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="E188" s="12"/>
       <c r="F188" s="13"/>
     </row>
-    <row r="189" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="189" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B189" s="6" t="s">
         <v>7</v>
       </c>
@@ -2651,8 +2651,8 @@
       <c r="E190" s="12"/>
       <c r="F190" s="13"/>
     </row>
-    <row r="191" spans="2:15" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="192" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:15" ht="10" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="192" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B192" s="3" t="s">
         <v>0</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="2:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B193" s="6" t="s">
         <v>1</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="194" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B194" s="6" t="s">
         <v>2</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="195" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="195" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B195" s="6" t="s">
         <v>3</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="196" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B196" s="6" t="s">
         <v>4</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="197" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B197" s="6" t="s">
         <v>5</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="198" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="198" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B198" s="6" t="s">
         <v>6</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="199" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="199" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B199" s="6" t="s">
         <v>7</v>
       </c>
@@ -2724,8 +2724,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="201" spans="2:19" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="202" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:19" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="202" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B202" s="3" t="s">
         <v>0</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B203" s="6" t="s">
         <v>1</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="204" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B204" s="6" t="s">
         <v>2</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="205" spans="2:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B205" s="6" t="s">
         <v>3</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="O205" s="5"/>
       <c r="S205" s="2"/>
     </row>
-    <row r="206" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="206" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B206" s="6" t="s">
         <v>4</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="207" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="B207" s="6" t="s">
         <v>5</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="208" spans="2:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:19" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B208" s="6" t="s">
         <v>6</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B209" s="6" t="s">
         <v>7</v>
       </c>
@@ -2800,8 +2800,8 @@
         <v>152</v>
       </c>
     </row>
-    <row r="211" spans="2:3" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:3" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="212" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B212" s="3" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B213" s="6" t="s">
         <v>1</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="214" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B214" s="6" t="s">
         <v>2</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B215" s="6" t="s">
         <v>3</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B216" s="6" t="s">
         <v>4</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B217" s="6" t="s">
         <v>5</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B218" s="6" t="s">
         <v>6</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B219" s="6" t="s">
         <v>7</v>
       </c>
@@ -2873,8 +2873,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="221" spans="2:3" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:3" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="222" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B222" s="3" t="s">
         <v>0</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="223" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B223" s="6" t="s">
         <v>1</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="B224" s="6" t="s">
         <v>2</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="225" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B225" s="6" t="s">
         <v>3</v>
       </c>
@@ -2908,7 +2908,7 @@
       <c r="M225" s="2"/>
       <c r="O225" s="5"/>
     </row>
-    <row r="226" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B226" s="6" t="s">
         <v>4</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="M226" s="2"/>
       <c r="O226" s="5"/>
     </row>
-    <row r="227" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B227" s="6" t="s">
         <v>5</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="M227" s="2"/>
       <c r="O227" s="5"/>
     </row>
-    <row r="228" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B228" s="6" t="s">
         <v>6</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="M228" s="2"/>
       <c r="O228" s="5"/>
     </row>
-    <row r="229" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B229" s="6" t="s">
         <v>7</v>
       </c>
@@ -2958,11 +2958,11 @@
       <c r="M230" s="2"/>
       <c r="O230" s="5"/>
     </row>
-    <row r="231" spans="2:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:15" ht="7.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M231" s="2"/>
       <c r="O231" s="5"/>
     </row>
-    <row r="232" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B232" s="3" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +2972,7 @@
       <c r="M232" s="2"/>
       <c r="O232" s="5"/>
     </row>
-    <row r="233" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B233" s="6" t="s">
         <v>1</v>
       </c>
@@ -2982,7 +2982,7 @@
       <c r="M233" s="2"/>
       <c r="O233" s="5"/>
     </row>
-    <row r="234" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B234" s="6" t="s">
         <v>2</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="M234" s="2"/>
       <c r="O234" s="5"/>
     </row>
-    <row r="235" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="235" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B235" s="6" t="s">
         <v>3</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="M235" s="2"/>
       <c r="O235" s="5"/>
     </row>
-    <row r="236" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B236" s="6" t="s">
         <v>4</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="M236" s="2"/>
       <c r="O236" s="5"/>
     </row>
-    <row r="237" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B237" s="6" t="s">
         <v>5</v>
       </c>
@@ -3022,7 +3022,7 @@
       <c r="M237" s="2"/>
       <c r="O237" s="5"/>
     </row>
-    <row r="238" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="238" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B238" s="6" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3032,7 @@
       <c r="M238" s="2"/>
       <c r="O238" s="5"/>
     </row>
-    <row r="239" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="239" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B239" s="6" t="s">
         <v>7</v>
       </c>
@@ -3052,11 +3052,11 @@
       <c r="M240" s="2"/>
       <c r="O240" s="5"/>
     </row>
-    <row r="241" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="241" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="M241" s="2"/>
       <c r="O241" s="5"/>
     </row>
-    <row r="242" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B242" s="3" t="s">
         <v>0</v>
       </c>
@@ -3066,7 +3066,7 @@
       <c r="M242" s="2"/>
       <c r="O242" s="5"/>
     </row>
-    <row r="243" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B243" s="6" t="s">
         <v>1</v>
       </c>
@@ -3076,7 +3076,7 @@
       <c r="M243" s="2"/>
       <c r="O243" s="5"/>
     </row>
-    <row r="244" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B244" s="6" t="s">
         <v>2</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="M244" s="2"/>
       <c r="O244" s="5"/>
     </row>
-    <row r="245" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B245" s="6" t="s">
         <v>3</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="M245" s="2"/>
       <c r="O245" s="5"/>
     </row>
-    <row r="246" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B246" s="6" t="s">
         <v>4</v>
       </c>
@@ -3106,7 +3106,7 @@
       <c r="M246" s="2"/>
       <c r="O246" s="5"/>
     </row>
-    <row r="247" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B247" s="6" t="s">
         <v>5</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="M247" s="2"/>
       <c r="O247" s="5"/>
     </row>
-    <row r="248" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B248" s="6" t="s">
         <v>6</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="M248" s="2"/>
       <c r="O248" s="5"/>
     </row>
-    <row r="249" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B249" s="6" t="s">
         <v>7</v>
       </c>
@@ -3146,11 +3146,11 @@
       <c r="M250" s="2"/>
       <c r="O250" s="5"/>
     </row>
-    <row r="251" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="251" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="M251" s="2"/>
       <c r="O251" s="5"/>
     </row>
-    <row r="252" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B252" s="3" t="s">
         <v>0</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="M252" s="2"/>
       <c r="O252" s="5"/>
     </row>
-    <row r="253" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B253" s="6" t="s">
         <v>1</v>
       </c>
@@ -3170,7 +3170,7 @@
       <c r="M253" s="2"/>
       <c r="O253" s="5"/>
     </row>
-    <row r="254" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B254" s="6" t="s">
         <v>2</v>
       </c>
@@ -3180,7 +3180,7 @@
       <c r="M254" s="2"/>
       <c r="O254" s="5"/>
     </row>
-    <row r="255" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B255" s="6" t="s">
         <v>3</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="M255" s="2"/>
       <c r="O255" s="5"/>
     </row>
-    <row r="256" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B256" s="6" t="s">
         <v>4</v>
       </c>
@@ -3200,7 +3200,7 @@
       <c r="M256" s="2"/>
       <c r="O256" s="5"/>
     </row>
-    <row r="257" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="257" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B257" s="6" t="s">
         <v>5</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="M257" s="2"/>
       <c r="O257" s="5"/>
     </row>
-    <row r="258" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B258" s="6" t="s">
         <v>6</v>
       </c>
@@ -3220,7 +3220,7 @@
       <c r="M258" s="2"/>
       <c r="O258" s="5"/>
     </row>
-    <row r="259" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="259" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B259" s="6" t="s">
         <v>7</v>
       </c>
@@ -3240,12 +3240,12 @@
       <c r="M260" s="2"/>
       <c r="O260" s="5"/>
     </row>
-    <row r="261" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="261" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="E261" s="5"/>
       <c r="M261" s="2"/>
       <c r="O261" s="5"/>
     </row>
-    <row r="262" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="262" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B262" s="3" t="s">
         <v>0</v>
       </c>
@@ -3256,7 +3256,7 @@
       <c r="M262" s="2"/>
       <c r="O262" s="5"/>
     </row>
-    <row r="263" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="263" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B263" s="6" t="s">
         <v>1</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="M263" s="2"/>
       <c r="O263" s="5"/>
     </row>
-    <row r="264" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="264" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B264" s="6" t="s">
         <v>2</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="M264" s="2"/>
       <c r="O264" s="5"/>
     </row>
-    <row r="265" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="265" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B265" s="6" t="s">
         <v>3</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="M265" s="2"/>
       <c r="O265" s="5"/>
     </row>
-    <row r="266" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B266" s="6" t="s">
         <v>4</v>
       </c>
@@ -3300,7 +3300,7 @@
       <c r="M266" s="2"/>
       <c r="O266" s="5"/>
     </row>
-    <row r="267" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="267" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B267" s="6" t="s">
         <v>5</v>
       </c>
@@ -3311,7 +3311,7 @@
       <c r="M267" s="2"/>
       <c r="O267" s="5"/>
     </row>
-    <row r="268" spans="2:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="268" spans="2:15" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B268" s="6" t="s">
         <v>6</v>
       </c>
@@ -3322,7 +3322,7 @@
       <c r="M268" s="2"/>
       <c r="O268" s="5"/>
     </row>
-    <row r="269" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="269" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B269" s="6" t="s">
         <v>7</v>
       </c>
@@ -3344,12 +3344,12 @@
       <c r="M270" s="2"/>
       <c r="O270" s="5"/>
     </row>
-    <row r="271" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="271" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="E271" s="5"/>
       <c r="M271" s="2"/>
       <c r="O271" s="5"/>
     </row>
-    <row r="272" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="272" spans="2:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="B272" s="3" t="s">
         <v>0</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="273" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="273" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B273" s="6" t="s">
         <v>1</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="274" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="274" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B274" s="6" t="s">
         <v>2</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="275" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="275" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B275" s="6" t="s">
         <v>3</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="276" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="276" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B276" s="6" t="s">
         <v>4</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="277" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B277" s="6" t="s">
         <v>5</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="278" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:5" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="B278" s="6" t="s">
         <v>6</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="279" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B279" s="6" t="s">
         <v>7</v>
       </c>
@@ -3421,10 +3421,10 @@
         <v>159</v>
       </c>
     </row>
-    <row r="281" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="281" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E281" s="5"/>
     </row>
-    <row r="282" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B282" s="3" t="s">
         <v>0</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="E282" s="5"/>
     </row>
-    <row r="283" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="283" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B283" s="6" t="s">
         <v>1</v>
       </c>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="E283" s="5"/>
     </row>
-    <row r="284" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B284" s="6" t="s">
         <v>2</v>
       </c>
@@ -3451,7 +3451,7 @@
       </c>
       <c r="E284" s="5"/>
     </row>
-    <row r="285" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B285" s="6" t="s">
         <v>3</v>
       </c>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="E285" s="5"/>
     </row>
-    <row r="286" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="286" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B286" s="6" t="s">
         <v>4</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="E286" s="5"/>
     </row>
-    <row r="287" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="287" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B287" s="6" t="s">
         <v>5</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="E287" s="5"/>
     </row>
-    <row r="288" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="288" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B288" s="6" t="s">
         <v>6</v>
       </c>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="E288" s="5"/>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B289" s="6" t="s">
         <v>7</v>
       </c>
@@ -3505,23 +3505,29 @@
       </c>
       <c r="E290" s="5"/>
     </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="291" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E291" s="5"/>
     </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="292" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E292" s="5"/>
     </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="293" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E293" s="5"/>
     </row>
-    <row r="294" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="294" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E294" s="5"/>
     </row>
-    <row r="295" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="295" spans="2:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="E295" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:C295" xr:uid="{293AA2FC-3EF2-4F89-B916-7D2D989016C7}"/>
+  <autoFilter ref="B1:C295" xr:uid="{293AA2FC-3EF2-4F89-B916-7D2D989016C7}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Sentiment           "/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>